<commit_message>
Modified crop inventory file. Restructured folders
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3634912-B293-4624-A171-AEBAEFABF1C9}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3682406D-560B-448F-9D96-4376C0775150}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="491">
   <si>
     <t>file_name</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>Cotton</t>
   </si>
   <si>
-    <t>crop_subtype</t>
-  </si>
-  <si>
     <t>Various</t>
   </si>
   <si>
@@ -1540,6 +1537,21 @@
   </si>
   <si>
     <t>../data/land_use/lu_Urban.tif</t>
+  </si>
+  <si>
+    <t>commodity_type</t>
+  </si>
+  <si>
+    <t>crop_class</t>
+  </si>
+  <si>
+    <t>crop_subclass</t>
+  </si>
+  <si>
+    <t>permanent</t>
+  </si>
+  <si>
+    <t>annual</t>
   </si>
 </sst>
 </file>
@@ -1673,7 +1685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1703,6 +1715,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1805,8 +1818,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{104850C8-860C-4F23-93B2-CD904150A6F6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="13" unboundColumnsRight="8">
-    <queryTableFields count="11">
+  <queryTableRefresh nextId="15" unboundColumnsRight="10">
+    <queryTableFields count="13">
       <queryTableField id="1" name="file_name" tableColumnId="1"/>
       <queryTableField id="2" name="land_use" tableColumnId="2"/>
       <queryTableField id="3" name="path" tableColumnId="3"/>
@@ -1814,6 +1827,8 @@
       <queryTableField id="5" dataBound="0" tableColumnId="5"/>
       <queryTableField id="6" dataBound="0" tableColumnId="6"/>
       <queryTableField id="7" dataBound="0" tableColumnId="7"/>
+      <queryTableField id="13" dataBound="0" tableColumnId="12"/>
+      <queryTableField id="14" dataBound="0" tableColumnId="13"/>
       <queryTableField id="8" dataBound="0" tableColumnId="8"/>
       <queryTableField id="9" dataBound="0" tableColumnId="9"/>
       <queryTableField id="11" dataBound="0" tableColumnId="10"/>
@@ -1824,17 +1839,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:K81" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:K81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{705AD7F1-810F-4078-AF9D-E2A5540C1883}" uniqueName="1" name="file_name" queryTableFieldId="1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{058DBECE-D8A6-44ED-99FF-D660796ED3BB}" uniqueName="2" name="land_use" queryTableFieldId="2" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{7DFC2AB1-8AD1-462B-A932-B862CB28BAB1}" uniqueName="3" name="path" queryTableFieldId="3" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{B2D579CF-A571-45E0-B50C-E961A8E35C10}" uniqueName="4" name="crop_name" queryTableFieldId="4" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{64E84341-910C-45DB-9CF2-A1479B33DB9F}" uniqueName="5" name="irrigation_type" queryTableFieldId="5" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{2F6D434D-16CF-4B4F-AB70-00F4EE5CC576}" uniqueName="6" name="on_off_field" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{21B7956E-4A5C-427A-B53C-1727078C89EA}" uniqueName="7" name="crop_type" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{A55D118B-687D-492C-A26A-CBF26CECBEF2}" uniqueName="8" name="crop_subtype" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{21B7956E-4A5C-427A-B53C-1727078C89EA}" uniqueName="7" name="commodity_type" queryTableFieldId="7" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{7A4FB457-40F4-4DD8-A0BB-88585C232B49}" uniqueName="12" name="crop_type" queryTableFieldId="13"/>
+    <tableColumn id="13" xr3:uid="{AEFE9D70-4CF9-44BD-B00B-BD26F54C2B75}" uniqueName="13" name="crop_class" queryTableFieldId="14"/>
+    <tableColumn id="8" xr3:uid="{A55D118B-687D-492C-A26A-CBF26CECBEF2}" uniqueName="8" name="crop_subclass" queryTableFieldId="8" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{1F7CC7C8-E38E-48A3-AE7F-C87CEFA067CE}" uniqueName="9" name="c_crop" queryTableFieldId="9" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{675905E3-F4F9-434F-8898-3F732502BE89}" uniqueName="10" name="c_res" queryTableFieldId="11" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{7F2A30B4-3EEF-48B3-B2C4-983D0B2C5ED4}" uniqueName="11" name="c_final" queryTableFieldId="12" dataDxfId="0">
@@ -2162,11 +2179,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:K82"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2178,9 +2193,11 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.36328125" customWidth="1"/>
+    <col min="10" max="10" width="21.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2200,30 +2217,36 @@
         <v>89</v>
       </c>
       <c r="G1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H1" t="s">
         <v>306</v>
       </c>
-      <c r="H1" t="s">
-        <v>312</v>
-      </c>
       <c r="I1" t="s">
-        <v>316</v>
+        <v>487</v>
       </c>
       <c r="J1" t="s">
+        <v>488</v>
+      </c>
+      <c r="K1" t="s">
+        <v>315</v>
+      </c>
+      <c r="L1" t="s">
+        <v>404</v>
+      </c>
+      <c r="M1" t="s">
         <v>405</v>
       </c>
-      <c r="K1" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -2235,31 +2258,34 @@
         <v>90</v>
       </c>
       <c r="G2" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" t="s">
+        <v>322</v>
+      </c>
+      <c r="J2" t="s">
         <v>323</v>
       </c>
-      <c r="H2" t="s">
-        <v>324</v>
-      </c>
-      <c r="I2">
+      <c r="K2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2271,31 +2297,34 @@
         <v>90</v>
       </c>
       <c r="G3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I3" t="s">
+        <v>322</v>
+      </c>
+      <c r="J3" t="s">
         <v>323</v>
       </c>
-      <c r="H3" t="s">
-        <v>324</v>
-      </c>
-      <c r="I3">
+      <c r="K3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -2307,31 +2336,34 @@
         <v>90</v>
       </c>
       <c r="G4" t="s">
+        <v>322</v>
+      </c>
+      <c r="I4" t="s">
+        <v>322</v>
+      </c>
+      <c r="J4" t="s">
         <v>323</v>
       </c>
-      <c r="H4" t="s">
-        <v>324</v>
-      </c>
-      <c r="I4">
+      <c r="K4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -2343,31 +2375,34 @@
         <v>90</v>
       </c>
       <c r="G5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I5" t="s">
+        <v>322</v>
+      </c>
+      <c r="J5" t="s">
         <v>323</v>
       </c>
-      <c r="H5" t="s">
-        <v>324</v>
-      </c>
-      <c r="I5">
+      <c r="K5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -2379,31 +2414,34 @@
         <v>90</v>
       </c>
       <c r="G6" t="s">
+        <v>322</v>
+      </c>
+      <c r="I6" t="s">
+        <v>322</v>
+      </c>
+      <c r="J6" t="s">
         <v>323</v>
       </c>
-      <c r="H6" t="s">
-        <v>324</v>
-      </c>
-      <c r="I6">
+      <c r="K6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2415,31 +2453,34 @@
         <v>90</v>
       </c>
       <c r="G7" t="s">
+        <v>322</v>
+      </c>
+      <c r="I7" t="s">
+        <v>322</v>
+      </c>
+      <c r="J7" t="s">
         <v>323</v>
       </c>
-      <c r="H7" t="s">
-        <v>324</v>
-      </c>
-      <c r="I7">
+      <c r="K7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -2451,31 +2492,34 @@
         <v>90</v>
       </c>
       <c r="G8" t="s">
+        <v>322</v>
+      </c>
+      <c r="I8" t="s">
+        <v>322</v>
+      </c>
+      <c r="J8" t="s">
         <v>323</v>
       </c>
-      <c r="H8" t="s">
-        <v>324</v>
-      </c>
-      <c r="I8">
+      <c r="K8">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2487,31 +2531,34 @@
         <v>90</v>
       </c>
       <c r="G9" t="s">
+        <v>322</v>
+      </c>
+      <c r="I9" t="s">
+        <v>322</v>
+      </c>
+      <c r="J9" t="s">
         <v>323</v>
       </c>
-      <c r="H9" t="s">
-        <v>324</v>
-      </c>
-      <c r="I9">
+      <c r="K9">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2525,29 +2572,32 @@
       <c r="G10" t="s">
         <v>11</v>
       </c>
-      <c r="H10" t="s">
-        <v>324</v>
-      </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>323</v>
+      </c>
+      <c r="K10">
         <v>0.01</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D11" t="s">
         <v>92</v>
@@ -2558,32 +2608,39 @@
       <c r="F11" t="s">
         <v>90</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H11" t="s">
+        <v>489</v>
+      </c>
+      <c r="I11" t="s">
         <v>307</v>
       </c>
-      <c r="H11" t="s">
-        <v>313</v>
-      </c>
-      <c r="I11">
+      <c r="J11" t="s">
+        <v>312</v>
+      </c>
+      <c r="K11">
         <v>0.15</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D12" t="s">
         <v>93</v>
@@ -2594,32 +2651,39 @@
       <c r="F12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H12" t="s">
+        <v>489</v>
+      </c>
+      <c r="I12" t="s">
         <v>307</v>
       </c>
-      <c r="H12" t="s">
-        <v>313</v>
-      </c>
-      <c r="I12">
+      <c r="J12" t="s">
+        <v>312</v>
+      </c>
+      <c r="K12">
         <v>0.15</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D13" t="s">
         <v>127</v>
@@ -2630,33 +2694,40 @@
       <c r="F13" t="s">
         <v>85</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H13" t="s">
+        <v>490</v>
+      </c>
+      <c r="I13" t="s">
         <v>308</v>
       </c>
-      <c r="H13" t="s">
-        <v>313</v>
-      </c>
-      <c r="I13">
+      <c r="J13" t="s">
+        <v>312</v>
+      </c>
+      <c r="K13">
         <v>0.2</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D14" t="s">
         <v>127</v>
@@ -2667,32 +2738,39 @@
       <c r="F14" t="s">
         <v>86</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H14" t="s">
+        <v>490</v>
+      </c>
+      <c r="I14" t="s">
         <v>308</v>
       </c>
-      <c r="H14" t="s">
-        <v>313</v>
-      </c>
-      <c r="I14">
+      <c r="J14" t="s">
+        <v>312</v>
+      </c>
+      <c r="K14">
         <v>0.2</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D15" t="s">
         <v>94</v>
@@ -2703,32 +2781,39 @@
       <c r="F15" t="s">
         <v>90</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H15" t="s">
+        <v>490</v>
+      </c>
+      <c r="I15" t="s">
         <v>309</v>
       </c>
-      <c r="H15" t="s">
-        <v>313</v>
-      </c>
-      <c r="I15">
+      <c r="J15" t="s">
+        <v>312</v>
+      </c>
+      <c r="K15">
         <v>0.34</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -2739,32 +2824,39 @@
       <c r="F16" t="s">
         <v>90</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H16" t="s">
+        <v>490</v>
+      </c>
+      <c r="I16" t="s">
         <v>310</v>
       </c>
-      <c r="H16" t="s">
-        <v>313</v>
-      </c>
-      <c r="I16">
+      <c r="J16" t="s">
+        <v>312</v>
+      </c>
+      <c r="K16">
         <v>0.5</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D17" t="s">
         <v>96</v>
@@ -2775,32 +2867,39 @@
       <c r="F17" t="s">
         <v>90</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H17" t="s">
+        <v>489</v>
+      </c>
+      <c r="I17" t="s">
         <v>307</v>
       </c>
-      <c r="H17" t="s">
-        <v>313</v>
-      </c>
-      <c r="I17">
+      <c r="J17" t="s">
+        <v>312</v>
+      </c>
+      <c r="K17">
         <v>0.15</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D18" t="s">
         <v>97</v>
@@ -2811,32 +2910,39 @@
       <c r="F18" t="s">
         <v>90</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H18" t="s">
+        <v>489</v>
+      </c>
+      <c r="I18" t="s">
         <v>307</v>
       </c>
-      <c r="H18" t="s">
-        <v>313</v>
-      </c>
-      <c r="I18">
+      <c r="J18" t="s">
+        <v>312</v>
+      </c>
+      <c r="K18">
         <v>0.15</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D19" t="s">
         <v>98</v>
@@ -2847,32 +2953,39 @@
       <c r="F19" t="s">
         <v>90</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H19" t="s">
+        <v>489</v>
+      </c>
+      <c r="I19" t="s">
         <v>98</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>98</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>0.2</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D20" t="s">
         <v>311</v>
@@ -2883,32 +2996,39 @@
       <c r="F20" t="s">
         <v>90</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H20" t="s">
+        <v>490</v>
+      </c>
+      <c r="I20" t="s">
         <v>311</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>311</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>0.4</v>
       </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D21" t="s">
         <v>100</v>
@@ -2919,32 +3039,39 @@
       <c r="F21" t="s">
         <v>90</v>
       </c>
-      <c r="G21" t="s">
-        <v>314</v>
+      <c r="G21" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
       </c>
       <c r="H21" t="s">
+        <v>489</v>
+      </c>
+      <c r="I21" t="s">
+        <v>313</v>
+      </c>
+      <c r="J21" t="s">
         <v>100</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>0.35</v>
       </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D22" t="s">
         <v>101</v>
@@ -2955,32 +3082,39 @@
       <c r="F22" t="s">
         <v>90</v>
       </c>
-      <c r="G22" t="s">
-        <v>315</v>
+      <c r="G22" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H22" t="s">
-        <v>313</v>
-      </c>
-      <c r="I22">
+        <v>490</v>
+      </c>
+      <c r="I22" t="s">
+        <v>314</v>
+      </c>
+      <c r="J22" t="s">
+        <v>312</v>
+      </c>
+      <c r="K22">
         <v>0.32</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.32</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D23" t="s">
         <v>138</v>
@@ -2991,33 +3125,40 @@
       <c r="F23" t="s">
         <v>85</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H23" t="s">
+        <v>490</v>
+      </c>
+      <c r="I23" t="s">
         <v>308</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>138</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>0.38</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D24" t="s">
         <v>138</v>
@@ -3028,32 +3169,39 @@
       <c r="F24" t="s">
         <v>86</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H24" t="s">
+        <v>490</v>
+      </c>
+      <c r="I24" t="s">
         <v>308</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>138</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>0.38</v>
       </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="K24">
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D25" t="s">
         <v>102</v>
@@ -3064,32 +3212,39 @@
       <c r="F25" t="s">
         <v>90</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H25" t="s">
+        <v>489</v>
+      </c>
+      <c r="I25" t="s">
         <v>307</v>
       </c>
-      <c r="H25" t="s">
-        <v>313</v>
-      </c>
-      <c r="I25">
+      <c r="J25" t="s">
+        <v>312</v>
+      </c>
+      <c r="K25">
         <v>0.15</v>
       </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D26" t="s">
         <v>103</v>
@@ -3100,32 +3255,39 @@
       <c r="F26" t="s">
         <v>90</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G26" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H26" t="s">
+        <v>489</v>
+      </c>
+      <c r="I26" t="s">
         <v>307</v>
       </c>
-      <c r="H26" t="s">
-        <v>313</v>
-      </c>
-      <c r="I26">
+      <c r="J26" t="s">
+        <v>312</v>
+      </c>
+      <c r="K26">
         <v>0.15</v>
       </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26">
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D27" t="s">
         <v>104</v>
@@ -3136,32 +3298,39 @@
       <c r="F27" t="s">
         <v>90</v>
       </c>
-      <c r="G27" t="s">
-        <v>317</v>
+      <c r="G27" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H27" t="s">
-        <v>313</v>
-      </c>
-      <c r="I27">
+        <v>490</v>
+      </c>
+      <c r="I27" t="s">
+        <v>316</v>
+      </c>
+      <c r="J27" t="s">
+        <v>312</v>
+      </c>
+      <c r="K27">
         <v>0.3</v>
       </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D28" t="s">
         <v>105</v>
@@ -3172,32 +3341,39 @@
       <c r="F28" t="s">
         <v>90</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H28" t="s">
+        <v>489</v>
+      </c>
+      <c r="I28" t="s">
         <v>307</v>
       </c>
-      <c r="H28" t="s">
-        <v>313</v>
-      </c>
-      <c r="I28">
+      <c r="J28" t="s">
+        <v>312</v>
+      </c>
+      <c r="K28">
         <v>0.15</v>
       </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D29" t="s">
         <v>106</v>
@@ -3208,32 +3384,39 @@
       <c r="F29" t="s">
         <v>90</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H29" t="s">
+        <v>490</v>
+      </c>
+      <c r="I29" t="s">
         <v>310</v>
       </c>
-      <c r="H29" t="s">
-        <v>313</v>
-      </c>
-      <c r="I29">
+      <c r="J29" t="s">
+        <v>312</v>
+      </c>
+      <c r="K29">
         <v>0.5</v>
       </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="K29">
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D30" t="s">
         <v>217</v>
@@ -3244,33 +3427,40 @@
       <c r="F30" t="s">
         <v>85</v>
       </c>
-      <c r="G30" t="s">
-        <v>318</v>
+      <c r="G30" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H30" t="s">
-        <v>313</v>
-      </c>
-      <c r="I30">
+        <v>490</v>
+      </c>
+      <c r="I30" t="s">
+        <v>317</v>
+      </c>
+      <c r="J30" t="s">
+        <v>312</v>
+      </c>
+      <c r="K30">
         <v>0.25</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D31" t="s">
         <v>217</v>
@@ -3281,32 +3471,39 @@
       <c r="F31" t="s">
         <v>86</v>
       </c>
-      <c r="G31" t="s">
-        <v>318</v>
+      <c r="G31" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H31" t="s">
-        <v>313</v>
-      </c>
-      <c r="I31">
+        <v>490</v>
+      </c>
+      <c r="I31" t="s">
+        <v>317</v>
+      </c>
+      <c r="J31" t="s">
+        <v>312</v>
+      </c>
+      <c r="K31">
         <v>0.25</v>
       </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="K31">
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D32" t="s">
         <v>107</v>
@@ -3317,32 +3514,39 @@
       <c r="F32" t="s">
         <v>90</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H32" t="s">
+        <v>490</v>
+      </c>
+      <c r="I32" t="s">
         <v>308</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>107</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>0.15</v>
       </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32">
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D33" t="s">
         <v>128</v>
@@ -3353,33 +3557,40 @@
       <c r="F33" t="s">
         <v>85</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H33" t="s">
+        <v>490</v>
+      </c>
+      <c r="I33" t="s">
+        <v>318</v>
+      </c>
+      <c r="J33" t="s">
         <v>319</v>
       </c>
-      <c r="H33" t="s">
-        <v>320</v>
-      </c>
-      <c r="I33">
+      <c r="K33">
         <v>0.1</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D34" t="s">
         <v>128</v>
@@ -3390,32 +3601,39 @@
       <c r="F34" t="s">
         <v>86</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H34" t="s">
+        <v>490</v>
+      </c>
+      <c r="I34" t="s">
+        <v>318</v>
+      </c>
+      <c r="J34" t="s">
         <v>319</v>
       </c>
-      <c r="H34" t="s">
-        <v>320</v>
-      </c>
-      <c r="I34">
+      <c r="K34">
         <v>0.1</v>
       </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-      <c r="K34">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D35" t="s">
         <v>108</v>
@@ -3426,32 +3644,39 @@
       <c r="F35" t="s">
         <v>90</v>
       </c>
-      <c r="G35" t="s">
-        <v>315</v>
+      <c r="G35" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H35" t="s">
-        <v>313</v>
-      </c>
-      <c r="I35">
+        <v>490</v>
+      </c>
+      <c r="I35" t="s">
+        <v>314</v>
+      </c>
+      <c r="J35" t="s">
+        <v>312</v>
+      </c>
+      <c r="K35">
         <v>0.32</v>
       </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="K35">
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.32</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D36" t="s">
         <v>109</v>
@@ -3462,32 +3687,39 @@
       <c r="F36" t="s">
         <v>90</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H36" t="s">
+        <v>490</v>
+      </c>
+      <c r="I36" t="s">
         <v>310</v>
       </c>
-      <c r="H36" t="s">
-        <v>313</v>
-      </c>
-      <c r="I36">
+      <c r="J36" t="s">
+        <v>312</v>
+      </c>
+      <c r="K36">
         <v>0.5</v>
       </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="K36">
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D37" t="s">
         <v>110</v>
@@ -3498,32 +3730,39 @@
       <c r="F37" t="s">
         <v>90</v>
       </c>
-      <c r="G37" t="s">
-        <v>321</v>
+      <c r="G37" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H37" t="s">
-        <v>321</v>
-      </c>
-      <c r="I37">
+        <v>490</v>
+      </c>
+      <c r="I37" t="s">
+        <v>320</v>
+      </c>
+      <c r="J37" t="s">
+        <v>320</v>
+      </c>
+      <c r="K37">
         <v>0.15</v>
       </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="K37">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D38" t="s">
         <v>111</v>
@@ -3534,32 +3773,39 @@
       <c r="F38" t="s">
         <v>90</v>
       </c>
-      <c r="G38" t="s">
-        <v>318</v>
+      <c r="G38" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H38" t="s">
-        <v>313</v>
-      </c>
-      <c r="I38">
+        <v>490</v>
+      </c>
+      <c r="I38" t="s">
+        <v>317</v>
+      </c>
+      <c r="J38" t="s">
+        <v>312</v>
+      </c>
+      <c r="K38">
         <v>0.25</v>
       </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="K38">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D39" t="s">
         <v>112</v>
@@ -3570,32 +3816,39 @@
       <c r="F39" t="s">
         <v>90</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H39" t="s">
+        <v>490</v>
+      </c>
+      <c r="I39" t="s">
         <v>310</v>
       </c>
-      <c r="H39" t="s">
-        <v>313</v>
-      </c>
-      <c r="I39">
+      <c r="J39" t="s">
+        <v>312</v>
+      </c>
+      <c r="K39">
         <v>0.5</v>
       </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D40" t="s">
         <v>113</v>
@@ -3606,32 +3859,39 @@
       <c r="F40" t="s">
         <v>90</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H40" t="s">
+        <v>490</v>
+      </c>
+      <c r="I40" t="s">
         <v>309</v>
       </c>
-      <c r="H40" t="s">
+      <c r="J40" t="s">
         <v>113</v>
       </c>
-      <c r="I40">
+      <c r="K40">
         <v>0.5</v>
       </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B41" t="s">
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D41" t="s">
         <v>114</v>
@@ -3642,32 +3902,39 @@
       <c r="F41" t="s">
         <v>90</v>
       </c>
-      <c r="G41" t="s">
-        <v>322</v>
+      <c r="G41" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
       </c>
       <c r="H41" t="s">
-        <v>313</v>
-      </c>
-      <c r="I41">
+        <v>490</v>
+      </c>
+      <c r="I41" t="s">
+        <v>321</v>
+      </c>
+      <c r="J41" t="s">
+        <v>312</v>
+      </c>
+      <c r="K41">
         <v>0.25</v>
       </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-      <c r="K41">
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B42" t="s">
         <v>43</v>
       </c>
       <c r="C42" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D42" t="s">
         <v>84</v>
@@ -3678,33 +3945,40 @@
       <c r="F42" t="s">
         <v>85</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G42" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H42" t="s">
+        <v>490</v>
+      </c>
+      <c r="I42" t="s">
         <v>308</v>
       </c>
-      <c r="H42" t="s">
-        <v>313</v>
-      </c>
-      <c r="I42">
+      <c r="J42" t="s">
+        <v>312</v>
+      </c>
+      <c r="K42">
         <v>0.2</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K42">
+      <c r="M42">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B43" t="s">
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D43" t="s">
         <v>84</v>
@@ -3715,32 +3989,39 @@
       <c r="F43" t="s">
         <v>86</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" t="str">
+        <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H43" t="s">
+        <v>490</v>
+      </c>
+      <c r="I43" t="s">
         <v>308</v>
       </c>
-      <c r="H43" t="s">
-        <v>313</v>
-      </c>
-      <c r="I43">
+      <c r="J43" t="s">
+        <v>312</v>
+      </c>
+      <c r="K43">
         <v>0.2</v>
       </c>
-      <c r="J43">
-        <v>1</v>
-      </c>
-      <c r="K43">
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D44" t="s">
         <v>115</v>
@@ -3752,31 +4033,34 @@
         <v>90</v>
       </c>
       <c r="G44" t="s">
+        <v>322</v>
+      </c>
+      <c r="I44" t="s">
+        <v>322</v>
+      </c>
+      <c r="J44" t="s">
         <v>323</v>
       </c>
-      <c r="H44" t="s">
-        <v>324</v>
-      </c>
-      <c r="I44">
+      <c r="K44">
         <v>1E-4</v>
       </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="K44">
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B45" t="s">
         <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D45" t="s">
         <v>116</v>
@@ -3788,31 +4072,34 @@
         <v>90</v>
       </c>
       <c r="G45" t="s">
+        <v>322</v>
+      </c>
+      <c r="I45" t="s">
+        <v>322</v>
+      </c>
+      <c r="J45" t="s">
         <v>323</v>
       </c>
-      <c r="H45" t="s">
-        <v>324</v>
-      </c>
-      <c r="I45">
+      <c r="K45">
         <v>1E-4</v>
       </c>
-      <c r="J45">
-        <v>1</v>
-      </c>
-      <c r="K45">
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D46" t="s">
         <v>117</v>
@@ -3824,31 +4111,34 @@
         <v>90</v>
       </c>
       <c r="G46" t="s">
+        <v>322</v>
+      </c>
+      <c r="I46" t="s">
+        <v>322</v>
+      </c>
+      <c r="J46" t="s">
         <v>323</v>
       </c>
-      <c r="H46" t="s">
-        <v>324</v>
-      </c>
-      <c r="I46">
+      <c r="K46">
         <v>1E-4</v>
       </c>
-      <c r="J46">
-        <v>1</v>
-      </c>
-      <c r="K46">
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D47" t="s">
         <v>118</v>
@@ -3860,31 +4150,34 @@
         <v>90</v>
       </c>
       <c r="G47" t="s">
+        <v>322</v>
+      </c>
+      <c r="I47" t="s">
+        <v>322</v>
+      </c>
+      <c r="J47" t="s">
         <v>323</v>
       </c>
-      <c r="H47" t="s">
-        <v>324</v>
-      </c>
-      <c r="I47">
+      <c r="K47">
         <v>1E-4</v>
       </c>
-      <c r="J47">
-        <v>1</v>
-      </c>
-      <c r="K47">
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D48" t="s">
         <v>119</v>
@@ -3896,31 +4189,34 @@
         <v>90</v>
       </c>
       <c r="G48" t="s">
+        <v>322</v>
+      </c>
+      <c r="I48" t="s">
+        <v>322</v>
+      </c>
+      <c r="J48" t="s">
         <v>323</v>
       </c>
-      <c r="H48" t="s">
-        <v>324</v>
-      </c>
-      <c r="I48">
+      <c r="K48">
         <v>1E-4</v>
       </c>
-      <c r="J48">
-        <v>1</v>
-      </c>
-      <c r="K48">
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D49" t="s">
         <v>120</v>
@@ -3932,31 +4228,34 @@
         <v>90</v>
       </c>
       <c r="G49" t="s">
+        <v>322</v>
+      </c>
+      <c r="I49" t="s">
+        <v>322</v>
+      </c>
+      <c r="J49" t="s">
         <v>323</v>
       </c>
-      <c r="H49" t="s">
-        <v>324</v>
-      </c>
-      <c r="I49">
+      <c r="K49">
         <v>1E-4</v>
       </c>
-      <c r="J49">
-        <v>1</v>
-      </c>
-      <c r="K49">
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
       </c>
       <c r="C50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D50" t="s">
         <v>121</v>
@@ -3968,31 +4267,34 @@
         <v>90</v>
       </c>
       <c r="G50" t="s">
+        <v>322</v>
+      </c>
+      <c r="I50" t="s">
+        <v>322</v>
+      </c>
+      <c r="J50" t="s">
         <v>323</v>
       </c>
-      <c r="H50" t="s">
-        <v>324</v>
-      </c>
-      <c r="I50">
+      <c r="K50">
         <v>1E-4</v>
       </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="K50">
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D51" t="s">
         <v>92</v>
@@ -4005,33 +4307,40 @@
       </c>
       <c r="G51" t="str">
         <f>+_xlfn.XLOOKUP($D51,$D$11:$D$43,G$11:G$43,"missing",0)</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H51" t="s">
+        <v>489</v>
+      </c>
+      <c r="I51" t="str">
+        <f>+_xlfn.XLOOKUP($D51,$D$11:$D$43,I$11:I$43,"missing",0)</f>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H51" t="str">
-        <f t="shared" ref="H51:I66" si="0">+_xlfn.XLOOKUP($D51,$D$11:$D$43,H$11:H$43,"missing",0)</f>
+      <c r="J51" t="str">
+        <f t="shared" ref="J51:K66" si="0">+_xlfn.XLOOKUP($D51,$D$11:$D$43,J$11:J$43,"missing",0)</f>
         <v>Various</v>
       </c>
-      <c r="I51">
+      <c r="K51">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-      <c r="K51">
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D52" t="s">
         <v>93</v>
@@ -4043,34 +4352,41 @@
         <v>90</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" ref="G52:I67" si="1">+_xlfn.XLOOKUP($D52,$D$11:$D$43,G$11:G$43,"missing",0)</f>
+        <f t="shared" ref="G52:K67" si="1">+_xlfn.XLOOKUP($D52,$D$11:$D$43,G$11:G$43,"missing",0)</f>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H52" t="s">
+        <v>489</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H52" t="str">
+      <c r="J52" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I52">
+      <c r="K52">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J52">
-        <v>1</v>
-      </c>
-      <c r="K52">
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D53" t="s">
         <v>127</v>
@@ -4083,34 +4399,41 @@
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H53" t="s">
+        <v>490</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="1"/>
         <v>Cereals</v>
       </c>
-      <c r="H53" t="str">
+      <c r="J53" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I53">
+      <c r="K53">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K53">
+      <c r="M53">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B54" t="s">
         <v>55</v>
       </c>
       <c r="C54" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D54" t="s">
         <v>127</v>
@@ -4123,33 +4446,40 @@
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H54" t="s">
+        <v>490</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
         <v>Cereals</v>
       </c>
-      <c r="H54" t="str">
+      <c r="J54" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I54">
+      <c r="K54">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J54">
-        <v>1</v>
-      </c>
-      <c r="K54">
+      <c r="L54">
+        <v>1</v>
+      </c>
+      <c r="M54">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D55" t="s">
         <v>96</v>
@@ -4162,33 +4492,40 @@
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H55" t="s">
+        <v>489</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H55" t="str">
+      <c r="J55" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I55">
+      <c r="K55">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J55">
-        <v>1</v>
-      </c>
-      <c r="K55">
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B56" t="s">
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D56" t="s">
         <v>97</v>
@@ -4201,33 +4538,40 @@
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H56" t="s">
+        <v>489</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H56" t="str">
+      <c r="J56" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I56">
+      <c r="K56">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J56">
-        <v>1</v>
-      </c>
-      <c r="K56">
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B57" t="s">
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D57" t="s">
         <v>98</v>
@@ -4240,33 +4584,40 @@
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H57" t="s">
+        <v>489</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
         <v>Coffee</v>
       </c>
-      <c r="H57" t="str">
+      <c r="J57" t="str">
         <f t="shared" si="0"/>
         <v>Coffee</v>
       </c>
-      <c r="I57">
+      <c r="K57">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="J57">
-        <v>1</v>
-      </c>
-      <c r="K57">
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B58" t="s">
         <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D58" t="s">
         <v>99</v>
@@ -4279,33 +4630,40 @@
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H58" t="s">
+        <v>490</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
         <v>Cotton</v>
       </c>
-      <c r="H58" t="str">
+      <c r="J58" t="str">
         <f t="shared" si="0"/>
         <v>Cotton</v>
       </c>
-      <c r="I58">
+      <c r="K58">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="J58">
-        <v>1</v>
-      </c>
-      <c r="K58">
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="M58">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B59" t="s">
         <v>60</v>
       </c>
       <c r="C59" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D59" t="s">
         <v>100</v>
@@ -4318,33 +4676,40 @@
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H59" t="s">
+        <v>489</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="1"/>
         <v>GrapesAndHops</v>
       </c>
-      <c r="H59" t="str">
+      <c r="J59" t="str">
         <f t="shared" si="0"/>
         <v>Grapes</v>
       </c>
-      <c r="I59">
-        <f>+_xlfn.XLOOKUP($D59,$D$11:$D$43,I$11:I$43,"missing",0)</f>
+      <c r="K59">
+        <f>+_xlfn.XLOOKUP($D59,$D$11:$D$43,K$11:K$43,"missing",0)</f>
         <v>0.35</v>
       </c>
-      <c r="J59">
-        <v>1</v>
-      </c>
-      <c r="K59">
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.35</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B60" t="s">
         <v>61</v>
       </c>
       <c r="C60" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D60" t="s">
         <v>101</v>
@@ -4357,33 +4722,40 @@
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H60" t="s">
+        <v>490</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="1"/>
         <v>Vegetables_Legume</v>
       </c>
-      <c r="H60" t="str">
+      <c r="J60" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I60">
+      <c r="K60">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-      <c r="K60">
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.32</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B61" t="s">
         <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D61" t="s">
         <v>138</v>
@@ -4396,34 +4768,41 @@
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H61" t="s">
+        <v>490</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="1"/>
         <v>Cereals</v>
       </c>
-      <c r="H61" t="str">
+      <c r="J61" t="str">
         <f t="shared" si="0"/>
         <v>Maize</v>
       </c>
-      <c r="I61">
+      <c r="K61">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="J61">
+      <c r="L61">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K61">
+      <c r="M61">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B62" t="s">
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D62" t="s">
         <v>138</v>
@@ -4436,33 +4815,40 @@
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H62" t="s">
+        <v>490</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="1"/>
         <v>Cereals</v>
       </c>
-      <c r="H62" t="str">
+      <c r="J62" t="str">
         <f t="shared" si="0"/>
         <v>Maize</v>
       </c>
-      <c r="I62">
+      <c r="K62">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="J62">
-        <v>1</v>
-      </c>
-      <c r="K62">
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="M62">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B63" t="s">
         <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D63" t="s">
         <v>102</v>
@@ -4475,33 +4861,40 @@
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H63" t="s">
+        <v>489</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H63" t="str">
+      <c r="J63" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I63">
+      <c r="K63">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J63">
-        <v>1</v>
-      </c>
-      <c r="K63">
+      <c r="L63">
+        <v>1</v>
+      </c>
+      <c r="M63">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B64" t="s">
         <v>65</v>
       </c>
       <c r="C64" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D64" t="s">
         <v>103</v>
@@ -4514,33 +4907,40 @@
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H64" t="s">
+        <v>489</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H64" t="str">
+      <c r="J64" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I64">
+      <c r="K64">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J64">
-        <v>1</v>
-      </c>
-      <c r="K64">
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B65" t="s">
         <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D65" t="s">
         <v>105</v>
@@ -4553,33 +4953,40 @@
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
+        <v>permanent_crop</v>
+      </c>
+      <c r="H65" t="s">
+        <v>489</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="1"/>
         <v>Fruit_Trees</v>
       </c>
-      <c r="H65" t="str">
+      <c r="J65" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I65">
+      <c r="K65">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-      <c r="K65">
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B66" t="s">
         <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D66" t="s">
         <v>106</v>
@@ -4592,33 +4999,40 @@
       </c>
       <c r="G66" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H66" t="s">
+        <v>490</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="1"/>
         <v>Vegetables_RootandTuber</v>
       </c>
-      <c r="H66" t="str">
+      <c r="J66" t="str">
         <f t="shared" si="0"/>
         <v>Various</v>
       </c>
-      <c r="I66">
+      <c r="K66">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J66">
-        <v>1</v>
-      </c>
-      <c r="K66">
+      <c r="L66">
+        <v>1</v>
+      </c>
+      <c r="M66">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B67" t="s">
         <v>68</v>
       </c>
       <c r="C67" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D67" t="s">
         <v>217</v>
@@ -4631,34 +5045,41 @@
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H67" t="s">
+        <v>490</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="1"/>
         <v>Oilseed</v>
       </c>
-      <c r="H67" t="str">
+      <c r="J67" t="str">
         <f t="shared" si="1"/>
         <v>Various</v>
       </c>
-      <c r="I67">
+      <c r="K67">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="J67">
+      <c r="L67">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K67">
+      <c r="M67">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.22</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B68" t="s">
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D68" t="s">
         <v>217</v>
@@ -4670,34 +5091,41 @@
         <v>86</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" ref="G68:I81" si="2">+_xlfn.XLOOKUP($D68,$D$11:$D$43,G$11:G$43,"missing",0)</f>
+        <f t="shared" ref="G68:K81" si="2">+_xlfn.XLOOKUP($D68,$D$11:$D$43,G$11:G$43,"missing",0)</f>
+        <v>annual_crop</v>
+      </c>
+      <c r="H68" t="s">
+        <v>490</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="2"/>
         <v>Oilseed</v>
       </c>
-      <c r="H68" t="str">
+      <c r="J68" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I68">
+      <c r="K68">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="J68">
-        <v>1</v>
-      </c>
-      <c r="K68">
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B69" t="s">
         <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D69" t="s">
         <v>107</v>
@@ -4710,33 +5138,40 @@
       </c>
       <c r="G69" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H69" t="s">
+        <v>490</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="2"/>
         <v>Cereals</v>
       </c>
-      <c r="H69" t="str">
+      <c r="J69" t="str">
         <f t="shared" si="2"/>
         <v>Rice</v>
       </c>
-      <c r="I69">
+      <c r="K69">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="J69">
-        <v>1</v>
-      </c>
-      <c r="K69">
+      <c r="L69">
+        <v>1</v>
+      </c>
+      <c r="M69">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B70" t="s">
         <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D70" t="s">
         <v>128</v>
@@ -4749,34 +5184,41 @@
       </c>
       <c r="G70" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H70" t="s">
+        <v>490</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Forage_Fodder_StrawOfCereal </v>
       </c>
-      <c r="H70" t="str">
+      <c r="J70" t="str">
         <f t="shared" si="2"/>
         <v>Mixed_Grasses</v>
       </c>
-      <c r="I70">
+      <c r="K70">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="J70">
+      <c r="L70">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K70">
+      <c r="M70">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B71" t="s">
         <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D71" t="s">
         <v>128</v>
@@ -4789,33 +5231,40 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H71" t="s">
+        <v>490</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Forage_Fodder_StrawOfCereal </v>
       </c>
-      <c r="H71" t="str">
+      <c r="J71" t="str">
         <f t="shared" si="2"/>
         <v>Mixed_Grasses</v>
       </c>
-      <c r="I71">
+      <c r="K71">
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="K71">
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B72" t="s">
         <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D72" t="s">
         <v>108</v>
@@ -4828,33 +5277,40 @@
       </c>
       <c r="G72" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H72" t="s">
+        <v>490</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="2"/>
         <v>Vegetables_Legume</v>
       </c>
-      <c r="H72" t="str">
+      <c r="J72" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I72">
+      <c r="K72">
         <f t="shared" si="2"/>
         <v>0.32</v>
       </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-      <c r="K72">
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.32</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B73" t="s">
         <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D73" t="s">
         <v>109</v>
@@ -4867,33 +5323,40 @@
       </c>
       <c r="G73" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H73" t="s">
+        <v>490</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="2"/>
         <v>Vegetables_RootandTuber</v>
       </c>
-      <c r="H73" t="str">
+      <c r="J73" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I73">
+      <c r="K73">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="J73">
-        <v>1</v>
-      </c>
-      <c r="K73">
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B74" t="s">
         <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D74" t="s">
         <v>110</v>
@@ -4906,33 +5369,40 @@
       </c>
       <c r="G74" t="str">
         <f t="shared" si="2"/>
-        <v>Shrub_Herbs_and_Spices</v>
-      </c>
-      <c r="H74" t="str">
+        <v>annual_crop</v>
+      </c>
+      <c r="H74" t="s">
+        <v>490</v>
+      </c>
+      <c r="I74" t="str">
         <f t="shared" si="2"/>
         <v>Shrub_Herbs_and_Spices</v>
       </c>
-      <c r="I74">
+      <c r="J74" t="str">
+        <f t="shared" si="2"/>
+        <v>Shrub_Herbs_and_Spices</v>
+      </c>
+      <c r="K74">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-      <c r="K74">
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.15</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B75" t="s">
         <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D75" t="s">
         <v>111</v>
@@ -4945,33 +5415,40 @@
       </c>
       <c r="G75" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H75" t="s">
+        <v>490</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="2"/>
         <v>Oilseed</v>
       </c>
-      <c r="H75" t="str">
+      <c r="J75" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I75">
+      <c r="K75">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="J75">
-        <v>1</v>
-      </c>
-      <c r="K75">
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B76" t="s">
         <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D76" t="s">
         <v>112</v>
@@ -4984,33 +5461,40 @@
       </c>
       <c r="G76" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H76" t="s">
+        <v>490</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="2"/>
         <v>Vegetables_RootandTuber</v>
       </c>
-      <c r="H76" t="str">
+      <c r="J76" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I76">
+      <c r="K76">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="J76">
-        <v>1</v>
-      </c>
-      <c r="K76">
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B77" t="s">
         <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D77" t="s">
         <v>113</v>
@@ -5023,33 +5507,40 @@
       </c>
       <c r="G77" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H77" t="s">
+        <v>490</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="2"/>
         <v>Vegetables_Leafy</v>
       </c>
-      <c r="H77" t="str">
+      <c r="J77" t="str">
         <f t="shared" si="2"/>
         <v>Tobacco</v>
       </c>
-      <c r="I77">
+      <c r="K77">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="J77">
-        <v>1</v>
-      </c>
-      <c r="K77">
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B78" t="s">
         <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D78" t="s">
         <v>114</v>
@@ -5062,33 +5553,40 @@
       </c>
       <c r="G78" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H78" t="s">
+        <v>490</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="2"/>
         <v>Vegetables_Fruiting</v>
       </c>
-      <c r="H78" t="str">
+      <c r="J78" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I78">
+      <c r="K78">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="J78">
-        <v>1</v>
-      </c>
-      <c r="K78">
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B79" t="s">
         <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D79" t="s">
         <v>84</v>
@@ -5101,34 +5599,41 @@
       </c>
       <c r="G79" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H79" t="s">
+        <v>490</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="2"/>
         <v>Cereals</v>
       </c>
-      <c r="H79" t="str">
+      <c r="J79" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I79">
+      <c r="K79">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="J79">
+      <c r="L79">
         <f>1-0.12</f>
         <v>0.88</v>
       </c>
-      <c r="K79">
+      <c r="M79">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B80" t="s">
         <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D80" t="s">
         <v>84</v>
@@ -5141,33 +5646,40 @@
       </c>
       <c r="G80" t="str">
         <f t="shared" si="2"/>
+        <v>annual_crop</v>
+      </c>
+      <c r="H80" t="s">
+        <v>490</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="2"/>
         <v>Cereals</v>
       </c>
-      <c r="H80" t="str">
+      <c r="J80" t="str">
         <f t="shared" si="2"/>
         <v>Various</v>
       </c>
-      <c r="I80">
+      <c r="K80">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="J80">
-        <v>1</v>
-      </c>
-      <c r="K80">
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B81" t="s">
         <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D81" t="s">
         <v>82</v>
@@ -5178,24 +5690,50 @@
       <c r="F81" t="s">
         <v>90</v>
       </c>
-      <c r="G81" t="str">
+      <c r="I81" t="str">
         <f t="shared" si="2"/>
         <v>missing</v>
       </c>
-      <c r="H81" t="str">
+      <c r="J81" t="str">
         <f t="shared" si="2"/>
         <v>missing</v>
       </c>
-      <c r="I81">
-        <v>1</v>
-      </c>
-      <c r="J81">
-        <v>1</v>
-      </c>
       <c r="K81">
-        <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A82" s="11"/>
+      <c r="B82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="J82" s="11"/>
+      <c r="K82" s="11"/>
+      <c r="L82" s="11"/>
+      <c r="M82" s="11"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="J83" s="11"/>
+      <c r="K83" s="11"/>
+      <c r="L83" s="11"/>
+      <c r="M83" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
forest  scenarios prepared. test running
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3682406D-560B-448F-9D96-4376C0775150}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{809590A3-7A90-4860-94D8-84489A3EBE07}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1685,7 +1685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1715,7 +1715,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1840,7 +1839,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
+  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Forest"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{705AD7F1-810F-4078-AF9D-E2A5540C1883}" uniqueName="1" name="file_name" queryTableFieldId="1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{058DBECE-D8A6-44ED-99FF-D660796ED3BB}" uniqueName="2" name="land_use" queryTableFieldId="2" dataDxfId="9"/>
@@ -2179,9 +2184,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
-  <dimension ref="A1:M83"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2550,7 +2557,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -2589,7 +2596,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -2632,7 +2639,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>334</v>
       </c>
@@ -2675,7 +2682,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>335</v>
       </c>
@@ -2719,7 +2726,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>336</v>
       </c>
@@ -2762,7 +2769,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -2805,7 +2812,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>338</v>
       </c>
@@ -2848,7 +2855,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>339</v>
       </c>
@@ -2891,7 +2898,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>340</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>341</v>
       </c>
@@ -2977,7 +2984,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>342</v>
       </c>
@@ -3020,7 +3027,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>343</v>
       </c>
@@ -3063,7 +3070,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>344</v>
       </c>
@@ -3106,7 +3113,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>345</v>
       </c>
@@ -3150,7 +3157,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>346</v>
       </c>
@@ -3193,7 +3200,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>347</v>
       </c>
@@ -3236,7 +3243,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>348</v>
       </c>
@@ -3279,7 +3286,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>349</v>
       </c>
@@ -3322,7 +3329,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -3365,7 +3372,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>351</v>
       </c>
@@ -3408,7 +3415,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>352</v>
       </c>
@@ -3452,7 +3459,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>353</v>
       </c>
@@ -3495,7 +3502,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -3538,7 +3545,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>355</v>
       </c>
@@ -3582,7 +3589,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>356</v>
       </c>
@@ -3625,7 +3632,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>357</v>
       </c>
@@ -3668,7 +3675,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>358</v>
       </c>
@@ -3711,7 +3718,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>359</v>
       </c>
@@ -3754,7 +3761,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>360</v>
       </c>
@@ -3797,7 +3804,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -3840,7 +3847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>362</v>
       </c>
@@ -3883,7 +3890,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>363</v>
       </c>
@@ -3926,7 +3933,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>364</v>
       </c>
@@ -3970,7 +3977,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>365</v>
       </c>
@@ -4286,7 +4293,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>373</v>
       </c>
@@ -4332,7 +4339,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>374</v>
       </c>
@@ -4378,7 +4385,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>375</v>
       </c>
@@ -4425,7 +4432,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>376</v>
       </c>
@@ -4471,7 +4478,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>377</v>
       </c>
@@ -4517,7 +4524,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -4563,7 +4570,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -4609,7 +4616,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>380</v>
       </c>
@@ -4655,7 +4662,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>381</v>
       </c>
@@ -4701,7 +4708,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>382</v>
       </c>
@@ -4747,7 +4754,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>383</v>
       </c>
@@ -4794,7 +4801,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -4840,7 +4847,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>385</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>386</v>
       </c>
@@ -4932,7 +4939,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>387</v>
       </c>
@@ -4978,7 +4985,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>388</v>
       </c>
@@ -5024,7 +5031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>389</v>
       </c>
@@ -5071,7 +5078,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>390</v>
       </c>
@@ -5117,7 +5124,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5163,7 +5170,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>392</v>
       </c>
@@ -5210,7 +5217,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>393</v>
       </c>
@@ -5256,7 +5263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>394</v>
       </c>
@@ -5302,7 +5309,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>395</v>
       </c>
@@ -5348,7 +5355,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>396</v>
       </c>
@@ -5394,7 +5401,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>397</v>
       </c>
@@ -5440,7 +5447,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>398</v>
       </c>
@@ -5486,7 +5493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>399</v>
       </c>
@@ -5532,7 +5539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>400</v>
       </c>
@@ -5578,7 +5585,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>401</v>
       </c>
@@ -5625,7 +5632,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>402</v>
       </c>
@@ -5671,7 +5678,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>403</v>
       </c>
@@ -5708,32 +5715,6 @@
         <f>+foreground_occupation_file_index[[#This Row],[c_res]]*foreground_occupation_file_index[[#This Row],[c_crop]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-      <c r="L82" s="11"/>
-      <c r="M82" s="11"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="11"/>
-      <c r="M83" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Kept creating residue stochastic calculations for rothC.
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{809590A3-7A90-4860-94D8-84489A3EBE07}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6419ED4D-C22B-4602-B92E-1684D86F0FD7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1842,7 +1842,7 @@
   <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
     <filterColumn colId="6">
       <filters>
-        <filter val="Forest"/>
+        <filter val="permanent_crop"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2245,7 +2245,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>324</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>325</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>326</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>331</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>334</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>339</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>340</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>341</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>343</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>347</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>348</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>366</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>367</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>369</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>370</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>371</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>372</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>373</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>374</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>377</v>
       </c>
@@ -4524,7 +4524,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>381</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>385</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>386</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>387</v>
       </c>

</xml_diff>

<commit_message>
finished running permanent crop soc model successfully
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6419ED4D-C22B-4602-B92E-1684D86F0FD7}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB623B91-D76E-415F-9BF9-FE96730CF47F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1839,13 +1839,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="permanent_crop"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{705AD7F1-810F-4078-AF9D-E2A5540C1883}" uniqueName="1" name="file_name" queryTableFieldId="1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{058DBECE-D8A6-44ED-99FF-D660796ED3BB}" uniqueName="2" name="land_use" queryTableFieldId="2" dataDxfId="9"/>
@@ -2186,7 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2245,7 +2239,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>324</v>
       </c>
@@ -2284,7 +2278,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>325</v>
       </c>
@@ -2323,7 +2317,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>326</v>
       </c>
@@ -2362,7 +2356,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -2401,7 +2395,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -2440,7 +2434,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -2479,7 +2473,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -2518,7 +2512,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>331</v>
       </c>
@@ -2557,7 +2551,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -2682,7 +2676,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>335</v>
       </c>
@@ -2726,7 +2720,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>336</v>
       </c>
@@ -2769,7 +2763,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -2812,7 +2806,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>338</v>
       </c>
@@ -2984,7 +2978,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>342</v>
       </c>
@@ -3070,7 +3064,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>344</v>
       </c>
@@ -3113,7 +3107,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>345</v>
       </c>
@@ -3157,7 +3151,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>346</v>
       </c>
@@ -3286,7 +3280,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>349</v>
       </c>
@@ -3372,7 +3366,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>351</v>
       </c>
@@ -3415,7 +3409,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>352</v>
       </c>
@@ -3459,7 +3453,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>353</v>
       </c>
@@ -3502,7 +3496,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -3545,7 +3539,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>355</v>
       </c>
@@ -3589,7 +3583,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>356</v>
       </c>
@@ -3632,7 +3626,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>357</v>
       </c>
@@ -3675,7 +3669,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>358</v>
       </c>
@@ -3718,7 +3712,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>359</v>
       </c>
@@ -3761,7 +3755,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>360</v>
       </c>
@@ -3804,7 +3798,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -3847,7 +3841,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>362</v>
       </c>
@@ -3890,7 +3884,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>363</v>
       </c>
@@ -3933,7 +3927,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>364</v>
       </c>
@@ -3977,7 +3971,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>365</v>
       </c>
@@ -4020,7 +4014,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>366</v>
       </c>
@@ -4059,7 +4053,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>367</v>
       </c>
@@ -4098,7 +4092,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -4137,7 +4131,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>369</v>
       </c>
@@ -4176,7 +4170,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>370</v>
       </c>
@@ -4215,7 +4209,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>371</v>
       </c>
@@ -4254,7 +4248,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>372</v>
       </c>
@@ -4385,7 +4379,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>375</v>
       </c>
@@ -4432,7 +4426,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>376</v>
       </c>
@@ -4616,7 +4610,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>380</v>
       </c>
@@ -4708,7 +4702,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>382</v>
       </c>
@@ -4754,7 +4748,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>383</v>
       </c>
@@ -4801,7 +4795,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -4985,7 +4979,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>388</v>
       </c>
@@ -5031,7 +5025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>389</v>
       </c>
@@ -5078,7 +5072,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>390</v>
       </c>
@@ -5124,7 +5118,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5170,7 +5164,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>392</v>
       </c>
@@ -5217,7 +5211,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>393</v>
       </c>
@@ -5263,7 +5257,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>394</v>
       </c>
@@ -5309,7 +5303,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>395</v>
       </c>
@@ -5355,7 +5349,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>396</v>
       </c>
@@ -5401,7 +5395,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>397</v>
       </c>
@@ -5447,7 +5441,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>398</v>
       </c>
@@ -5493,7 +5487,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>399</v>
       </c>
@@ -5539,7 +5533,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>400</v>
       </c>
@@ -5585,7 +5579,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>401</v>
       </c>
@@ -5632,7 +5626,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>402</v>
       </c>
@@ -5678,7 +5672,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>403</v>
       </c>

</xml_diff>

<commit_message>
fixed some crops annual vs perennial classification
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5252FFCB-0D4B-4296-9DBB-6B3A784BA013}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C3B9869-D6E2-4592-8BA8-D946D215A130}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1839,13 +1839,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="annual_crop"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{705AD7F1-810F-4078-AF9D-E2A5540C1883}" uniqueName="1" name="file_name" queryTableFieldId="1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{058DBECE-D8A6-44ED-99FF-D660796ED3BB}" uniqueName="2" name="land_use" queryTableFieldId="2" dataDxfId="9"/>
@@ -2186,9 +2180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2245,7 +2237,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>324</v>
       </c>
@@ -2284,7 +2276,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>325</v>
       </c>
@@ -2323,7 +2315,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>326</v>
       </c>
@@ -2362,7 +2354,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -2401,7 +2393,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -2440,7 +2432,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -2479,7 +2471,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>331</v>
       </c>
@@ -2557,7 +2549,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -2596,7 +2588,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -2639,7 +2631,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>334</v>
       </c>
@@ -2855,7 +2847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>339</v>
       </c>
@@ -2898,7 +2890,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>340</v>
       </c>
@@ -2941,7 +2933,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>341</v>
       </c>
@@ -3027,7 +3019,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>343</v>
       </c>
@@ -3200,7 +3192,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>347</v>
       </c>
@@ -3243,7 +3235,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>348</v>
       </c>
@@ -3329,7 +3321,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -3739,10 +3731,10 @@
       </c>
       <c r="G37" t="str">
         <f>+foreground_occupation_file_index[[#This Row],[crop_type]]&amp;"_crop"</f>
-        <v>annual_crop</v>
+        <v>permanent_crop</v>
       </c>
       <c r="H37" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I37" t="s">
         <v>320</v>
@@ -4020,7 +4012,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>366</v>
       </c>
@@ -4059,7 +4051,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>367</v>
       </c>
@@ -4098,7 +4090,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -4137,7 +4129,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>369</v>
       </c>
@@ -4176,7 +4168,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>370</v>
       </c>
@@ -4215,7 +4207,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>371</v>
       </c>
@@ -4254,7 +4246,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>372</v>
       </c>
@@ -4293,7 +4285,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>373</v>
       </c>
@@ -4339,7 +4331,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>374</v>
       </c>
@@ -4478,7 +4470,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>377</v>
       </c>
@@ -4524,7 +4516,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -4570,7 +4562,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -4662,7 +4654,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>381</v>
       </c>
@@ -4847,7 +4839,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>385</v>
       </c>
@@ -4893,7 +4885,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>386</v>
       </c>
@@ -4939,7 +4931,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>387</v>
       </c>
@@ -5376,10 +5368,10 @@
       </c>
       <c r="G74" t="str">
         <f t="shared" si="2"/>
-        <v>annual_crop</v>
+        <v>permanent_crop</v>
       </c>
       <c r="H74" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I74" t="str">
         <f t="shared" si="2"/>
@@ -5678,7 +5670,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>403</v>
       </c>

</xml_diff>

<commit_message>
Updated SOC maps test
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C3B9869-D6E2-4592-8BA8-D946D215A130}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A22A7B-BA43-4431-ACBC-A397DDAA5F56}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1839,7 +1839,14 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}"/>
+  <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="off"/>
+        <filter val="on"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{705AD7F1-810F-4078-AF9D-E2A5540C1883}" uniqueName="1" name="file_name" queryTableFieldId="1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{058DBECE-D8A6-44ED-99FF-D660796ED3BB}" uniqueName="2" name="land_use" queryTableFieldId="2" dataDxfId="9"/>
@@ -2180,7 +2187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2237,7 +2246,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>324</v>
       </c>
@@ -2276,7 +2285,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>325</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>326</v>
       </c>
@@ -2354,7 +2363,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>327</v>
       </c>
@@ -2393,7 +2402,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>328</v>
       </c>
@@ -2432,7 +2441,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>330</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>331</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>332</v>
       </c>
@@ -2588,7 +2597,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>333</v>
       </c>
@@ -2631,7 +2640,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>334</v>
       </c>
@@ -2761,7 +2770,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>337</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>338</v>
       </c>
@@ -2847,7 +2856,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>339</v>
       </c>
@@ -2890,7 +2899,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>340</v>
       </c>
@@ -2933,7 +2942,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>341</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>342</v>
       </c>
@@ -3019,7 +3028,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>343</v>
       </c>
@@ -3062,7 +3071,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>344</v>
       </c>
@@ -3192,7 +3201,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>347</v>
       </c>
@@ -3235,7 +3244,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>348</v>
       </c>
@@ -3278,7 +3287,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>349</v>
       </c>
@@ -3321,7 +3330,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -3364,7 +3373,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>351</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -3624,7 +3633,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>357</v>
       </c>
@@ -3667,7 +3676,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>358</v>
       </c>
@@ -3710,7 +3719,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>359</v>
       </c>
@@ -3753,7 +3762,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>360</v>
       </c>
@@ -3796,7 +3805,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>361</v>
       </c>
@@ -3839,7 +3848,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>362</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>363</v>
       </c>
@@ -4012,7 +4021,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>366</v>
       </c>
@@ -4051,7 +4060,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>367</v>
       </c>
@@ -4090,7 +4099,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -4129,7 +4138,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>369</v>
       </c>
@@ -4168,7 +4177,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>370</v>
       </c>
@@ -4207,7 +4216,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>371</v>
       </c>
@@ -4246,7 +4255,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>372</v>
       </c>
@@ -4285,7 +4294,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>373</v>
       </c>
@@ -4331,7 +4340,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>374</v>
       </c>
@@ -4470,7 +4479,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>377</v>
       </c>
@@ -4516,7 +4525,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>378</v>
       </c>
@@ -4562,7 +4571,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>379</v>
       </c>
@@ -4608,7 +4617,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>380</v>
       </c>
@@ -4654,7 +4663,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>381</v>
       </c>
@@ -4700,7 +4709,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>382</v>
       </c>
@@ -4839,7 +4848,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>385</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>386</v>
       </c>
@@ -4931,7 +4940,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>387</v>
       </c>
@@ -4977,7 +4986,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>388</v>
       </c>
@@ -5116,7 +5125,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5255,7 +5264,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>394</v>
       </c>
@@ -5301,7 +5310,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>395</v>
       </c>
@@ -5347,7 +5356,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>396</v>
       </c>
@@ -5393,7 +5402,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>397</v>
       </c>
@@ -5439,7 +5448,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>398</v>
       </c>
@@ -5485,7 +5494,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>399</v>
       </c>
@@ -5531,7 +5540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>400</v>
       </c>
@@ -5670,7 +5679,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>403</v>
       </c>

</xml_diff>

<commit_message>
All soil erosion regional averages tested successfully
</commit_message>
<xml_diff>
--- a/data/crops/lu_c_factor_inventory.xlsx
+++ b/data/crops/lu_c_factor_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A22A7B-BA43-4431-ACBC-A397DDAA5F56}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{AA2EB21E-9C36-413E-A92A-3D12D76AAA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFE3B18A-B01B-4791-895C-7BFAF4541078}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F9D02B0-B27B-4DAB-8C90-F4F799F4886A}"/>
   </bookViews>
@@ -1840,10 +1840,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}" name="foreground_occupation_file_index" displayName="foreground_occupation_file_index" ref="A1:M81" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:M81" xr:uid="{B91ACB39-A6C6-4049-8B69-94BB57FE429E}">
-    <filterColumn colId="5">
+    <filterColumn colId="3">
       <filters>
-        <filter val="off"/>
-        <filter val="on"/>
+        <filter val="Wheat"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2187,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E97CAB-CCC3-4E9F-B107-D69EEAD4EC67}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2683,7 +2682,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>335</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>336</v>
       </c>
@@ -3114,7 +3113,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>345</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>346</v>
       </c>
@@ -3416,7 +3415,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>352</v>
       </c>
@@ -3460,7 +3459,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>353</v>
       </c>
@@ -3546,7 +3545,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>355</v>
       </c>
@@ -3590,7 +3589,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>356</v>
       </c>
@@ -4386,7 +4385,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>375</v>
       </c>
@@ -4433,7 +4432,7 @@
         <v>0.17600000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>376</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>383</v>
       </c>
@@ -4802,7 +4801,7 @@
         <v>0.33440000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -5032,7 +5031,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>389</v>
       </c>
@@ -5079,7 +5078,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>390</v>
       </c>
@@ -5171,7 +5170,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>392</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>8.8000000000000009E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>393</v>
       </c>

</xml_diff>